<commit_message>
hands per ton update
</commit_message>
<xml_diff>
--- a/HandsPerTon.xlsx
+++ b/HandsPerTon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jashfaque\Desktop\dashboardSoft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF79702-D655-4FC6-BDD6-86759B11063B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2C35B4-90A3-4C09-BFA8-DCFC4588B838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hands Per Ton" sheetId="1" r:id="rId1"/>
@@ -488,16 +488,16 @@
   <dimension ref="A1:P173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O153" sqref="O153"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.109375" style="3" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
file uploader conditional statement update
</commit_message>
<xml_diff>
--- a/HandsPerTon.xlsx
+++ b/HandsPerTon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jashfaque\Desktop\dashboardSoft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB11F46-2C7B-4FFE-A41D-8296C61E8844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE0B196-C54C-4E6C-8B33-1B337FFF4116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hands Per Ton" sheetId="1" r:id="rId1"/>
@@ -526,12 +526,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O742"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H543" sqref="H543"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -601,7 +601,7 @@
         <v>19.671150971599399</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -625,7 +625,7 @@
         <v>16.346153846153847</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -649,7 +649,7 @@
         <v>14.967320261437909</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -673,7 +673,7 @@
         <v>14.84375</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -697,7 +697,7 @@
         <v>15.17241379310345</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -721,7 +721,7 @@
         <v>15.144508670520231</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -745,7 +745,7 @@
         <v>15.070821529745043</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -769,7 +769,7 @@
         <v>26.495726495726498</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -793,7 +793,7 @@
         <v>16.022443890274314</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -817,7 +817,7 @@
         <v>15.857988165680474</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -841,7 +841,7 @@
         <v>14.829545454545453</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -865,7 +865,7 @@
         <v>15.141242937853107</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -889,7 +889,7 @@
         <v>16.246153846153845</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -913,7 +913,7 @@
         <v>16.196319018404907</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -937,7 +937,7 @@
         <v>17.974683544303797</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -961,7 +961,7 @@
         <v>18.447204968944099</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -985,7 +985,7 @@
         <v>18.333333333333336</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>17.764705882352942</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>16.811594202898551</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>21.071428571428569</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>17.664670658682635</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>18.691588785046729</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>18.253012048192769</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>16.420454545454543</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>16.460674157303369</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>17.329376854599406</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>17.434210526315791</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>16.040548598688133</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>16.477272727272727</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>17.543859649122805</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>16.927374301675979</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>17.514124293785311</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>35.384615384615387</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>15.81005586592179</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>17.55952380952381</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>17.314285714285713</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>17.89473684210526</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>17.376093294460642</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>18.363636363636363</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>14.191616766467066</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>15.243902439024392</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>14.357541899441342</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>15.085714285714285</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>14.931350114416476</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>23.055555555555554</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>15.314285714285715</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="H50"/>
     </row>
-    <row r="51" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>14.309392265193368</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>14.767441860465118</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>15.502958579881659</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>16.263079222720478</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>26</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>17.516339869281044</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>18.788713007570543</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>26</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>18.06930693069307</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>16.705202312138727</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>17.253731343283583</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>21.875</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>17.106842737094837</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>17.125748502994014</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>16.959064327485379</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>16.779661016949152</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>16.206896551724139</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>16.571428571428573</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>17.564102564102566</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>18.741721854304636</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>26</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>17.950310559006208</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>26</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>18.303030303030305</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>26</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>18.708509354254677</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>26</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>27.428571428571427</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -2340,7 +2340,7 @@
       </c>
       <c r="H75"/>
     </row>
-    <row r="76" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>26</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>26</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>18.143712574850301</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>18.143712574850301</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>26</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>18.650306748466257</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>26</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>35.778389374177337</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>26</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>24.58566567884974</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>22.31813875144752</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>26</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>23.691404272552393</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>26</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>26.021934197407777</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>24.71153846153846</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>26</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>25.193608469757866</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>23.209736767619589</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>26</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>26.269509782369749</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>26</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>24.402440244024401</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>26</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>25.45419216943554</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>26</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>27.30019797853496</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>26</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>24.047529234251229</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>26</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>23.640441039058121</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>26</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>22.298911600743295</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>26</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>26.796116504854368</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>26</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>26.774133778024826</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>26</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>28.145542079437089</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>26</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>28.032090608777725</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>26</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>28.5410657355397</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>26</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>27.068761922063764</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>26</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>27.202996789154479</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>26</v>
       </c>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="H102"/>
     </row>
-    <row r="103" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>26</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>28.507960014809328</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>26</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>27.662133407345731</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>26</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>28.178063331803582</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>26</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>29.139871382636656</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>26</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>28.267014568384429</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>26</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>30.87912087912088</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>26</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>28.53437094682231</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>26</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>29.411764705882355</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>26</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>28.737864077669901</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>26</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>29.400235201881614</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>26</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>34.847186518137676</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>26</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>25.970207761662092</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>26</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>27.027027027027028</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>26</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>27.921894160928211</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>26</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>30.104443989350809</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>26</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>28.571428571428573</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>26</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>28.565987430965528</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>26</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>22.648401826484019</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>26</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>26</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>25.137837585272404</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>26</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>24.543223343332425</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>26</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>24.098536237058191</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>26</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>27.437155119558554</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>26</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>24.80592486838583</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>26</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>26</v>
       </c>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="H128"/>
     </row>
-    <row r="129" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>26</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>24.098536237058191</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>26</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>25.025208543404528</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>26</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>24.333093006488824</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>26</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>27.605099568011802</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>26</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>28.269717302826972</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>26</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>29.557191517415667</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>26</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>29.19191919191919</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>26</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>28.71189773844641</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>26</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>29.552238805970148</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>26</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>29.610914603335019</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>26</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>32.529444756029164</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>26</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>24.866948063864928</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>26</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>27.960364956342588</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>26</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>27.205743434725107</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>26</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>29.083224313172991</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>26</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>27.22200846479415</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>26</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>25.858814647036617</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>26</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>26.7343155429798</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>26</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>28.529411764705884</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>26</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>27.051811095827603</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>26</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>26.144937708369891</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>26</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>27.49745393945005</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>26</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>31.584309730005092</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>26</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>24.662102861154995</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>26</v>
       </c>
@@ -4203,7 +4203,7 @@
       </c>
       <c r="H153"/>
     </row>
-    <row r="154" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>26</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>26</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>27.316985214569058</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>26</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>26.389130813447135</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>26</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>27.250431465164866</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>26</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>35.75586229835357</v>
       </c>
     </row>
-    <row r="159" spans="1:13" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>26</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>23.4375</v>
       </c>
     </row>
-    <row r="160" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>26</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>26</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>26</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>26</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>26</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>26</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:15" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>26</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:15" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>26</v>
       </c>
@@ -4589,7 +4589,7 @@
       </c>
       <c r="O167" s="3"/>
     </row>
-    <row r="168" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>26</v>
       </c>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="O168" s="3"/>
     </row>
-    <row r="169" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>26</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>26</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>26</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>22.727272727272727</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>26</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>26.405228758169933</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>26</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>27.875507442489852</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>26</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>25.289925946625679</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>26</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>31.130268199233715</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>26</v>
       </c>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="M176" s="4"/>
     </row>
-    <row r="177" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>26</v>
       </c>
@@ -4841,7 +4841,7 @@
       </c>
       <c r="M177" s="4"/>
     </row>
-    <row r="178" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>26</v>
       </c>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="M178" s="4"/>
     </row>
-    <row r="179" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>26</v>
       </c>
@@ -4891,7 +4891,7 @@
       </c>
       <c r="M179" s="4"/>
     </row>
-    <row r="180" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>26</v>
       </c>
@@ -4913,7 +4913,7 @@
       <c r="H180"/>
       <c r="M180" s="4"/>
     </row>
-    <row r="181" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>26</v>
       </c>
@@ -4938,7 +4938,7 @@
       </c>
       <c r="M181" s="4"/>
     </row>
-    <row r="182" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>26</v>
       </c>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="M182" s="4"/>
     </row>
-    <row r="183" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>26</v>
       </c>
@@ -4988,7 +4988,7 @@
       </c>
       <c r="M183" s="4"/>
     </row>
-    <row r="184" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>26</v>
       </c>
@@ -5013,7 +5013,7 @@
       </c>
       <c r="M184" s="4"/>
     </row>
-    <row r="185" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>26</v>
       </c>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="M185" s="4"/>
     </row>
-    <row r="186" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>26</v>
       </c>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="M186" s="4"/>
     </row>
-    <row r="187" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>26</v>
       </c>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="M187" s="4"/>
     </row>
-    <row r="188" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>26</v>
       </c>
@@ -5113,7 +5113,7 @@
       </c>
       <c r="M188" s="4"/>
     </row>
-    <row r="189" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>26</v>
       </c>
@@ -5138,7 +5138,7 @@
       </c>
       <c r="M189" s="4"/>
     </row>
-    <row r="190" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>26</v>
       </c>
@@ -5163,7 +5163,7 @@
       </c>
       <c r="M190" s="4"/>
     </row>
-    <row r="191" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>26</v>
       </c>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="M191" s="4"/>
     </row>
-    <row r="192" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>26</v>
       </c>
@@ -5213,7 +5213,7 @@
       </c>
       <c r="M192" s="4"/>
     </row>
-    <row r="193" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>26</v>
       </c>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="M193" s="4"/>
     </row>
-    <row r="194" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>26</v>
       </c>
@@ -5263,7 +5263,7 @@
       </c>
       <c r="M194" s="4"/>
     </row>
-    <row r="195" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>26</v>
       </c>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="M195" s="4"/>
     </row>
-    <row r="196" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>26</v>
       </c>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="M196" s="4"/>
     </row>
-    <row r="197" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>26</v>
       </c>
@@ -5338,7 +5338,7 @@
       </c>
       <c r="M197" s="4"/>
     </row>
-    <row r="198" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>26</v>
       </c>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="M198" s="4"/>
     </row>
-    <row r="199" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>26</v>
       </c>
@@ -5388,7 +5388,7 @@
       </c>
       <c r="M199" s="4"/>
     </row>
-    <row r="200" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>26</v>
       </c>
@@ -5413,7 +5413,7 @@
       </c>
       <c r="M200" s="4"/>
     </row>
-    <row r="201" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>26</v>
       </c>
@@ -5438,7 +5438,7 @@
       </c>
       <c r="M201" s="4"/>
     </row>
-    <row r="202" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>26</v>
       </c>
@@ -5463,7 +5463,7 @@
       </c>
       <c r="M202" s="4"/>
     </row>
-    <row r="203" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>26</v>
       </c>
@@ -5488,7 +5488,7 @@
       </c>
       <c r="M203" s="4"/>
     </row>
-    <row r="204" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>26</v>
       </c>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="M204" s="4"/>
     </row>
-    <row r="205" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>26</v>
       </c>
@@ -5538,7 +5538,7 @@
       </c>
       <c r="M205" s="4"/>
     </row>
-    <row r="206" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>26</v>
       </c>
@@ -5560,7 +5560,7 @@
       <c r="H206"/>
       <c r="M206" s="4"/>
     </row>
-    <row r="207" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>26</v>
       </c>
@@ -5585,7 +5585,7 @@
       </c>
       <c r="M207" s="4"/>
     </row>
-    <row r="208" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>26</v>
       </c>
@@ -5610,7 +5610,7 @@
       </c>
       <c r="M208" s="4"/>
     </row>
-    <row r="209" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>26</v>
       </c>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="M209" s="4"/>
     </row>
-    <row r="210" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>26</v>
       </c>
@@ -5660,7 +5660,7 @@
       </c>
       <c r="M210" s="4"/>
     </row>
-    <row r="211" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>26</v>
       </c>
@@ -5685,7 +5685,7 @@
       </c>
       <c r="M211" s="4"/>
     </row>
-    <row r="212" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>26</v>
       </c>
@@ -5710,7 +5710,7 @@
       </c>
       <c r="M212" s="4"/>
     </row>
-    <row r="213" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>26</v>
       </c>
@@ -5735,7 +5735,7 @@
       </c>
       <c r="M213" s="4"/>
     </row>
-    <row r="214" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>26</v>
       </c>
@@ -5760,7 +5760,7 @@
       </c>
       <c r="M214" s="4"/>
     </row>
-    <row r="215" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>26</v>
       </c>
@@ -5785,7 +5785,7 @@
       </c>
       <c r="M215" s="4"/>
     </row>
-    <row r="216" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>26</v>
       </c>
@@ -5810,7 +5810,7 @@
       </c>
       <c r="M216" s="4"/>
     </row>
-    <row r="217" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>26</v>
       </c>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="M217" s="4"/>
     </row>
-    <row r="218" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>26</v>
       </c>
@@ -5860,7 +5860,7 @@
       </c>
       <c r="M218" s="4"/>
     </row>
-    <row r="219" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>26</v>
       </c>
@@ -5885,7 +5885,7 @@
       </c>
       <c r="M219" s="4"/>
     </row>
-    <row r="220" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>26</v>
       </c>
@@ -5910,7 +5910,7 @@
       </c>
       <c r="M220" s="4"/>
     </row>
-    <row r="221" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>26</v>
       </c>
@@ -5935,7 +5935,7 @@
       </c>
       <c r="M221" s="4"/>
     </row>
-    <row r="222" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>26</v>
       </c>
@@ -5960,7 +5960,7 @@
       </c>
       <c r="M222" s="4"/>
     </row>
-    <row r="223" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>26</v>
       </c>
@@ -5985,7 +5985,7 @@
       </c>
       <c r="M223" s="4"/>
     </row>
-    <row r="224" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>26</v>
       </c>
@@ -6010,7 +6010,7 @@
       </c>
       <c r="M224" s="4"/>
     </row>
-    <row r="225" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>26</v>
       </c>
@@ -6035,7 +6035,7 @@
       </c>
       <c r="M225" s="4"/>
     </row>
-    <row r="226" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>26</v>
       </c>
@@ -6060,7 +6060,7 @@
       </c>
       <c r="M226" s="4"/>
     </row>
-    <row r="227" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>26</v>
       </c>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="M227" s="4"/>
     </row>
-    <row r="228" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>26</v>
       </c>
@@ -6110,7 +6110,7 @@
       </c>
       <c r="M228" s="4"/>
     </row>
-    <row r="229" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>26</v>
       </c>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="M229" s="4"/>
     </row>
-    <row r="230" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>26</v>
       </c>
@@ -6160,7 +6160,7 @@
       </c>
       <c r="M230" s="4"/>
     </row>
-    <row r="231" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>26</v>
       </c>
@@ -6182,7 +6182,7 @@
       <c r="H231"/>
       <c r="M231" s="4"/>
     </row>
-    <row r="232" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>26</v>
       </c>
@@ -6207,7 +6207,7 @@
       </c>
       <c r="M232" s="4"/>
     </row>
-    <row r="233" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>26</v>
       </c>
@@ -6232,7 +6232,7 @@
       </c>
       <c r="M233" s="4"/>
     </row>
-    <row r="234" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>26</v>
       </c>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="M234" s="4"/>
     </row>
-    <row r="235" spans="1:13" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>26</v>
       </c>
@@ -6282,7 +6282,7 @@
       </c>
       <c r="M235" s="4"/>
     </row>
-    <row r="236" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>27</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>26.088141134800082</v>
       </c>
     </row>
-    <row r="237" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>27</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>25.620783694560071</v>
       </c>
     </row>
-    <row r="238" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>27</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>26.469390525315596</v>
       </c>
     </row>
-    <row r="239" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>27</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>26.84843847812478</v>
       </c>
     </row>
-    <row r="240" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>27</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>29.32898829802992</v>
       </c>
     </row>
-    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>27</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>27.70485007599834</v>
       </c>
     </row>
-    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>27</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>26.55337227827934</v>
       </c>
     </row>
-    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>27</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>24.815871541370846</v>
       </c>
     </row>
-    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>27</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>25.021570319240723</v>
       </c>
     </row>
-    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>27</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>24.526198439241917</v>
       </c>
     </row>
-    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>27</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>24.03876809283938</v>
       </c>
     </row>
-    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>27</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>24.778981446893287</v>
       </c>
     </row>
-    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>27</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>24.778981446893287</v>
       </c>
     </row>
-    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>27</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>22.907601740465829</v>
       </c>
     </row>
-    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>27</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>25.849030661350202</v>
       </c>
     </row>
-    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>27</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>25.609035393000198</v>
       </c>
     </row>
-    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>27</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>24.754370294755645</v>
       </c>
     </row>
-    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>27</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>25.467440361057381</v>
       </c>
     </row>
-    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>27</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>25.209542230818826</v>
       </c>
     </row>
-    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>27</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>25.6608639587363</v>
       </c>
     </row>
-    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>27</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>25.615502024022827</v>
       </c>
     </row>
-    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>27</v>
       </c>
@@ -6807,7 +6807,7 @@
       </c>
       <c r="H257" s="5"/>
     </row>
-    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>27</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>25.443525475093125</v>
       </c>
     </row>
-    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>27</v>
       </c>
@@ -6855,7 +6855,7 @@
         <v>25.303011370735973</v>
       </c>
     </row>
-    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>27</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>27.035916326799107</v>
       </c>
     </row>
-    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>27</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>27.783669141039237</v>
       </c>
     </row>
-    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>27</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>24.662001494666757</v>
       </c>
     </row>
-    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>27</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>25.151311365164762</v>
       </c>
     </row>
-    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>27</v>
       </c>
@@ -6975,7 +6975,7 @@
         <v>25.961472070703582</v>
       </c>
     </row>
-    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>27</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>26.417436887846602</v>
       </c>
     </row>
-    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>27</v>
       </c>
@@ -7023,7 +7023,7 @@
         <v>25.627191799298625</v>
       </c>
     </row>
-    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>27</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>25.483655770513675</v>
       </c>
     </row>
-    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>27</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>24.197332260875392</v>
       </c>
     </row>
-    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>27</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>25.123284019725443</v>
       </c>
     </row>
-    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>27</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>24.088625531366741</v>
       </c>
     </row>
-    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>27</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>24.806701030927837</v>
       </c>
     </row>
-    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>27</v>
       </c>
@@ -7167,7 +7167,7 @@
         <v>23.925537231384308</v>
       </c>
     </row>
-    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>27</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>23.925537231384308</v>
       </c>
     </row>
-    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>27</v>
       </c>
@@ -7215,7 +7215,7 @@
         <v>23.527209186220666</v>
       </c>
     </row>
-    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>27</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>24.2000873199027</v>
       </c>
     </row>
-    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>27</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>24.891220885589966</v>
       </c>
     </row>
-    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>27</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>25.121763650346065</v>
       </c>
     </row>
-    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>27</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>25.107282392877732</v>
       </c>
     </row>
-    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>27</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>23.826298597322744</v>
       </c>
     </row>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>27</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>24.787036443988985</v>
       </c>
     </row>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>27</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>25.520833333333336</v>
       </c>
     </row>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>27</v>
       </c>
@@ -7404,7 +7404,7 @@
       </c>
       <c r="H282" s="5"/>
     </row>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>27</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>24.337244676227726</v>
       </c>
     </row>
-    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>27</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>25.049726504226751</v>
       </c>
     </row>
-    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>27</v>
       </c>
@@ -7476,7 +7476,7 @@
         <v>25.958441230341691</v>
       </c>
     </row>
-    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>27</v>
       </c>
@@ -7500,7 +7500,7 @@
         <v>19.431675720852486</v>
       </c>
     </row>
-    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>27</v>
       </c>
@@ -7524,7 +7524,7 @@
         <v>21.881533101045296</v>
       </c>
     </row>
-    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>27</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>21.957726246665299</v>
       </c>
     </row>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>27</v>
       </c>
@@ -7572,7 +7572,7 @@
         <v>21.70412378351887</v>
       </c>
     </row>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>27</v>
       </c>
@@ -7596,7 +7596,7 @@
         <v>22.157517221788225</v>
       </c>
     </row>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>27</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>20.980445410103204</v>
       </c>
     </row>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>27</v>
       </c>
@@ -7644,7 +7644,7 @@
         <v>21.467499667685765</v>
       </c>
     </row>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>27</v>
       </c>
@@ -7668,7 +7668,7 @@
         <v>21.044944566155479</v>
       </c>
     </row>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>27</v>
       </c>
@@ -7692,7 +7692,7 @@
         <v>21.248162501670453</v>
       </c>
     </row>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>27</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>20.180528691166991</v>
       </c>
     </row>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>27</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>20.967218435572867</v>
       </c>
     </row>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>27</v>
       </c>
@@ -7764,7 +7764,7 @@
         <v>20.173630628942604</v>
       </c>
     </row>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>27</v>
       </c>
@@ -7788,7 +7788,7 @@
         <v>20.173630628942604</v>
       </c>
     </row>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>27</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>19.512817242698635</v>
       </c>
     </row>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>27</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>19.7613721103654</v>
       </c>
     </row>
-    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>27</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>20.368946963873942</v>
       </c>
     </row>
-    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>27</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>20.965036769449103</v>
       </c>
     </row>
-    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>27</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>22.083277903418917</v>
       </c>
     </row>
-    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>27</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>21.019023546627643</v>
       </c>
     </row>
-    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>27</v>
       </c>
@@ -7956,7 +7956,7 @@
         <v>20.885991752028733</v>
       </c>
     </row>
-    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>27</v>
       </c>
@@ -7977,7 +7977,7 @@
       </c>
       <c r="H306" s="5"/>
     </row>
-    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>27</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>21.969295923769192</v>
       </c>
     </row>
-    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>27</v>
       </c>
@@ -8025,7 +8025,7 @@
         <v>21.168501270110074</v>
       </c>
     </row>
-    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>27</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>21.218715995647443</v>
       </c>
     </row>
-    <row r="310" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>27</v>
       </c>
@@ -8073,7 +8073,7 @@
         <v>21.047917599641739</v>
       </c>
     </row>
-    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>27</v>
       </c>
@@ -8097,7 +8097,7 @@
         <v>24.246818108587078</v>
       </c>
     </row>
-    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>27</v>
       </c>
@@ -8121,7 +8121,7 @@
         <v>23.269342641070391</v>
       </c>
     </row>
-    <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>27</v>
       </c>
@@ -8145,7 +8145,7 @@
         <v>21.04596882664768</v>
       </c>
     </row>
-    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>27</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>21.947326416600159</v>
       </c>
     </row>
-    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>27</v>
       </c>
@@ -8193,7 +8193,7 @@
         <v>22.416534181240063</v>
       </c>
     </row>
-    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>27</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>22.527560313149063</v>
       </c>
     </row>
-    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>27</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>22.239810051444401</v>
       </c>
     </row>
-    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>27</v>
       </c>
@@ -8265,7 +8265,7 @@
         <v>21.545015155238797</v>
       </c>
     </row>
-    <row r="319" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>27</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>20.893141945773525</v>
       </c>
     </row>
-    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>27</v>
       </c>
@@ -8313,7 +8313,7 @@
         <v>22.055298066165896</v>
       </c>
     </row>
-    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>27</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>21.562050790608527</v>
       </c>
     </row>
-    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>27</v>
       </c>
@@ -8361,7 +8361,7 @@
         <v>21.978887663463052</v>
       </c>
     </row>
-    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>27</v>
       </c>
@@ -8385,7 +8385,7 @@
         <v>21.978887663463052</v>
       </c>
     </row>
-    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>27</v>
       </c>
@@ -8409,7 +8409,7 @@
         <v>22.627737226277372</v>
       </c>
     </row>
-    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>27</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>21.980676328502415</v>
       </c>
     </row>
-    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>27</v>
       </c>
@@ -8457,7 +8457,7 @@
         <v>21.05428548982638</v>
       </c>
     </row>
-    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>27</v>
       </c>
@@ -8481,7 +8481,7 @@
         <v>23.084828840224525</v>
       </c>
     </row>
-    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>27</v>
       </c>
@@ -8505,7 +8505,7 @@
         <v>23.311512054925753</v>
       </c>
     </row>
-    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>27</v>
       </c>
@@ -8529,7 +8529,7 @@
         <v>22.433338655596359</v>
       </c>
     </row>
-    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>27</v>
       </c>
@@ -8553,7 +8553,7 @@
         <v>23.151844164138591</v>
       </c>
     </row>
-    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>27</v>
       </c>
@@ -8577,7 +8577,7 @@
         <v>23.674770825029892</v>
       </c>
     </row>
-    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>27</v>
       </c>
@@ -8598,7 +8598,7 @@
       </c>
       <c r="H332" s="5"/>
     </row>
-    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>27</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>21.769149541060841</v>
       </c>
     </row>
-    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>27</v>
       </c>
@@ -8646,7 +8646,7 @@
         <v>21.229753105834252</v>
       </c>
     </row>
-    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>27</v>
       </c>
@@ -8670,7 +8670,7 @@
         <v>21.761658031088082</v>
       </c>
     </row>
-    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>27</v>
       </c>
@@ -8694,7 +8694,7 @@
         <v>23.015873015873016</v>
       </c>
     </row>
-    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>27</v>
       </c>
@@ -8718,7 +8718,7 @@
         <v>22.310126582278482</v>
       </c>
     </row>
-    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>27</v>
       </c>
@@ -8742,7 +8742,7 @@
         <v>21.43314139475368</v>
       </c>
     </row>
-    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>27</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>22.31107556977209</v>
       </c>
     </row>
-    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>27</v>
       </c>
@@ -8790,7 +8790,7 @@
         <v>22.009569377990431</v>
       </c>
     </row>
-    <row r="341" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>27</v>
       </c>
@@ -8814,7 +8814,7 @@
         <v>22.348152286694869</v>
       </c>
     </row>
-    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>27</v>
       </c>
@@ -8838,7 +8838,7 @@
         <v>21.499404998016658</v>
       </c>
     </row>
-    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>27</v>
       </c>
@@ -8862,7 +8862,7 @@
         <v>21.663504111321949</v>
       </c>
     </row>
-    <row r="344" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>27</v>
       </c>
@@ -8886,7 +8886,7 @@
         <v>21.780756342747726</v>
       </c>
     </row>
-    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>27</v>
       </c>
@@ -8910,7 +8910,7 @@
         <v>22.908684546615579</v>
       </c>
     </row>
-    <row r="346" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>27</v>
       </c>
@@ -8934,7 +8934,7 @@
         <v>23.020551218735065</v>
       </c>
     </row>
-    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>27</v>
       </c>
@@ -8958,7 +8958,7 @@
         <v>22.655758338577723</v>
       </c>
     </row>
-    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>27</v>
       </c>
@@ -8982,7 +8982,7 @@
         <v>22.655758338577723</v>
       </c>
     </row>
-    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>27</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>22.260407716941341</v>
       </c>
     </row>
-    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>27</v>
       </c>
@@ -9030,7 +9030,7 @@
         <v>22.239747634069403</v>
       </c>
     </row>
-    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>27</v>
       </c>
@@ -9054,7 +9054,7 @@
         <v>21.467327199811276</v>
       </c>
     </row>
-    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>27</v>
       </c>
@@ -9078,7 +9078,7 @@
         <v>22.914171656686626</v>
       </c>
     </row>
-    <row r="353" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>27</v>
       </c>
@@ -9102,7 +9102,7 @@
         <v>22.701927672454993</v>
       </c>
     </row>
-    <row r="354" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>27</v>
       </c>
@@ -9126,7 +9126,7 @@
         <v>22.064680579894855</v>
       </c>
     </row>
-    <row r="355" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>27</v>
       </c>
@@ -9150,7 +9150,7 @@
         <v>22.064680579894855</v>
       </c>
     </row>
-    <row r="356" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>27</v>
       </c>
@@ -9174,7 +9174,7 @@
         <v>23.334712453454696</v>
       </c>
     </row>
-    <row r="357" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>27</v>
       </c>
@@ -9195,7 +9195,7 @@
       </c>
       <c r="H357" s="5"/>
     </row>
-    <row r="358" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>27</v>
       </c>
@@ -9219,7 +9219,7 @@
         <v>21.796407185628741</v>
       </c>
     </row>
-    <row r="359" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>27</v>
       </c>
@@ -9243,7 +9243,7 @@
         <v>22.466216216216218</v>
       </c>
     </row>
-    <row r="360" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>27</v>
       </c>
@@ -9267,7 +9267,7 @@
         <v>21.425170607840023</v>
       </c>
     </row>
-    <row r="361" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>27</v>
       </c>
@@ -9291,7 +9291,7 @@
         <v>23.777961888980943</v>
       </c>
     </row>
-    <row r="362" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>27</v>
       </c>
@@ -9315,7 +9315,7 @@
         <v>20.502431118314426</v>
       </c>
     </row>
-    <row r="363" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>27</v>
       </c>
@@ -9339,7 +9339,7 @@
         <v>20.762395149904492</v>
       </c>
     </row>
-    <row r="364" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>27</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>22.026431718061673</v>
       </c>
     </row>
-    <row r="365" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>27</v>
       </c>
@@ -9387,7 +9387,7 @@
         <v>21.708155225882159</v>
       </c>
     </row>
-    <row r="366" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>27</v>
       </c>
@@ -9411,7 +9411,7 @@
         <v>21.458160729080365</v>
       </c>
     </row>
-    <row r="367" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>27</v>
       </c>
@@ -9435,7 +9435,7 @@
         <v>20.391177694548482</v>
       </c>
     </row>
-    <row r="368" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>27</v>
       </c>
@@ -9459,7 +9459,7 @@
         <v>20.964703955450002</v>
       </c>
     </row>
-    <row r="369" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>27</v>
       </c>
@@ -9483,7 +9483,7 @@
         <v>20.53520899021748</v>
       </c>
     </row>
-    <row r="370" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>27</v>
       </c>
@@ -9507,7 +9507,7 @@
         <v>20.791033866645009</v>
       </c>
     </row>
-    <row r="371" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>27</v>
       </c>
@@ -9531,7 +9531,7 @@
         <v>20.893603342976533</v>
       </c>
     </row>
-    <row r="372" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>27</v>
       </c>
@@ -9555,7 +9555,7 @@
         <v>20.228462636839602</v>
       </c>
     </row>
-    <row r="373" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>27</v>
       </c>
@@ -9579,7 +9579,7 @@
         <v>20.228462636839602</v>
       </c>
     </row>
-    <row r="374" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>27</v>
       </c>
@@ -9603,7 +9603,7 @@
         <v>18.54043392504931</v>
       </c>
     </row>
-    <row r="375" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>27</v>
       </c>
@@ -9627,7 +9627,7 @@
         <v>18.381475292432562</v>
       </c>
     </row>
-    <row r="376" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>27</v>
       </c>
@@ -9651,7 +9651,7 @@
         <v>18.713634219216857</v>
       </c>
     </row>
-    <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>27</v>
       </c>
@@ -9675,7 +9675,7 @@
         <v>19.085487077534793</v>
       </c>
     </row>
-    <row r="378" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>27</v>
       </c>
@@ -9699,7 +9699,7 @@
         <v>19.674520281758561</v>
       </c>
     </row>
-    <row r="379" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>27</v>
       </c>
@@ -9723,7 +9723,7 @@
         <v>20.241276010039673</v>
       </c>
     </row>
-    <row r="380" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>27</v>
       </c>
@@ -9747,7 +9747,7 @@
         <v>19.674520281758561</v>
       </c>
     </row>
-    <row r="381" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>27</v>
       </c>
@@ -9768,7 +9768,7 @@
       </c>
       <c r="H381" s="5"/>
     </row>
-    <row r="382" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>27</v>
       </c>
@@ -9792,7 +9792,7 @@
         <v>19.104084321475625</v>
       </c>
     </row>
-    <row r="383" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>27</v>
       </c>
@@ -9816,7 +9816,7 @@
         <v>18.456238208514478</v>
       </c>
     </row>
-    <row r="384" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>27</v>
       </c>
@@ -9840,7 +9840,7 @@
         <v>18.43817787418655</v>
       </c>
     </row>
-    <row r="385" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>27</v>
       </c>
@@ -9864,7 +9864,7 @@
         <v>19.749089437474705</v>
       </c>
     </row>
-    <row r="386" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>27</v>
       </c>
@@ -9888,7 +9888,7 @@
         <v>29.203001419590347</v>
       </c>
     </row>
-    <row r="387" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>27</v>
       </c>
@@ -9912,7 +9912,7 @@
         <v>28.80065830076116</v>
       </c>
     </row>
-    <row r="388" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>27</v>
       </c>
@@ -9936,7 +9936,7 @@
         <v>30.096887239744383</v>
       </c>
     </row>
-    <row r="389" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>27</v>
       </c>
@@ -9960,7 +9960,7 @@
         <v>38.671165325720217</v>
       </c>
     </row>
-    <row r="390" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>27</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>29.758277473085517</v>
       </c>
     </row>
-    <row r="391" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>27</v>
       </c>
@@ -10008,7 +10008,7 @@
         <v>30.235839548478129</v>
       </c>
     </row>
-    <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>27</v>
       </c>
@@ -10032,7 +10032,7 @@
         <v>31.108364235681911</v>
       </c>
     </row>
-    <row r="393" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>27</v>
       </c>
@@ -10056,7 +10056,7 @@
         <v>29.185078614736408</v>
       </c>
     </row>
-    <row r="394" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>27</v>
       </c>
@@ -10080,7 +10080,7 @@
         <v>28.448792174086641</v>
       </c>
     </row>
-    <row r="395" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>27</v>
       </c>
@@ -10104,7 +10104,7 @@
         <v>29.38783811267033</v>
       </c>
     </row>
-    <row r="396" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>27</v>
       </c>
@@ -10128,7 +10128,7 @@
         <v>30.501969498030501</v>
       </c>
     </row>
-    <row r="397" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>27</v>
       </c>
@@ -10152,7 +10152,7 @@
         <v>29.928172386272948</v>
       </c>
     </row>
-    <row r="398" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>27</v>
       </c>
@@ -10176,7 +10176,7 @@
         <v>29.928172386272948</v>
       </c>
     </row>
-    <row r="399" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>27</v>
       </c>
@@ -10200,7 +10200,7 @@
         <v>26.782035434693036</v>
       </c>
     </row>
-    <row r="400" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>27</v>
       </c>
@@ -10224,7 +10224,7 @@
         <v>27.045908183632736</v>
       </c>
     </row>
-    <row r="401" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>27</v>
       </c>
@@ -10248,7 +10248,7 @@
         <v>27.434158020750203</v>
       </c>
     </row>
-    <row r="402" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>27</v>
       </c>
@@ -10272,7 +10272,7 @@
         <v>28.088764494202319</v>
       </c>
     </row>
-    <row r="403" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>27</v>
       </c>
@@ -10296,7 +10296,7 @@
         <v>27.668383318186407</v>
       </c>
     </row>
-    <row r="404" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>27</v>
       </c>
@@ -10320,7 +10320,7 @@
         <v>26.355649803089971</v>
       </c>
     </row>
-    <row r="405" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>27</v>
       </c>
@@ -10344,7 +10344,7 @@
         <v>27.870342320508936</v>
       </c>
     </row>
-    <row r="406" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>27</v>
       </c>
@@ -10368,7 +10368,7 @@
         <v>28.95345330250327</v>
       </c>
     </row>
-    <row r="407" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>27</v>
       </c>
@@ -10389,7 +10389,7 @@
       </c>
       <c r="H407" s="5"/>
     </row>
-    <row r="408" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>27</v>
       </c>
@@ -10413,7 +10413,7 @@
         <v>26.811237062592411</v>
       </c>
     </row>
-    <row r="409" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>27</v>
       </c>
@@ -10437,7 +10437,7 @@
         <v>28.292488543534567</v>
       </c>
     </row>
-    <row r="410" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>27</v>
       </c>
@@ -10461,7 +10461,7 @@
         <v>28.879784151094235</v>
       </c>
     </row>
-    <row r="411" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>27</v>
       </c>
@@ -10485,7 +10485,7 @@
         <v>29.491696024157019</v>
       </c>
     </row>
-    <row r="412" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>27</v>
       </c>
@@ -10509,7 +10509,7 @@
         <v>27.671177539890934</v>
       </c>
     </row>
-    <row r="413" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>27</v>
       </c>
@@ -10533,7 +10533,7 @@
         <v>27.666799840191768</v>
       </c>
     </row>
-    <row r="414" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>27</v>
       </c>
@@ -10557,7 +10557,7 @@
         <v>27.891632510246925</v>
       </c>
     </row>
-    <row r="415" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>27</v>
       </c>
@@ -10581,7 +10581,7 @@
         <v>28.986971013028988</v>
       </c>
     </row>
-    <row r="416" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>27</v>
       </c>
@@ -10605,7 +10605,7 @@
         <v>28.658847526772057</v>
       </c>
     </row>
-    <row r="417" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>27</v>
       </c>
@@ -10629,7 +10629,7 @@
         <v>28.482910253847692</v>
       </c>
     </row>
-    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>27</v>
       </c>
@@ -10653,7 +10653,7 @@
         <v>25.579536370903281</v>
       </c>
     </row>
-    <row r="419" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>27</v>
       </c>
@@ -10677,7 +10677,7 @@
         <v>28.026790314270993</v>
       </c>
     </row>
-    <row r="420" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>27</v>
       </c>
@@ -10701,7 +10701,7 @@
         <v>26.722504736264831</v>
       </c>
     </row>
-    <row r="421" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>27</v>
       </c>
@@ -10725,7 +10725,7 @@
         <v>26.198714780029658</v>
       </c>
     </row>
-    <row r="422" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>27</v>
       </c>
@@ -10749,7 +10749,7 @@
         <v>28.508109197139117</v>
       </c>
     </row>
-    <row r="423" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>27</v>
       </c>
@@ -10773,7 +10773,7 @@
         <v>28.508109197139117</v>
       </c>
     </row>
-    <row r="424" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>27</v>
       </c>
@@ -10797,7 +10797,7 @@
         <v>29.293450232078388</v>
       </c>
     </row>
-    <row r="425" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>27</v>
       </c>
@@ -10821,7 +10821,7 @@
         <v>29.933830479991595</v>
       </c>
     </row>
-    <row r="426" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>27</v>
       </c>
@@ -10845,7 +10845,7 @@
         <v>28.642714570858285</v>
       </c>
     </row>
-    <row r="427" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>27</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>29.051987767584098</v>
       </c>
     </row>
-    <row r="428" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>27</v>
       </c>
@@ -10893,7 +10893,7 @@
         <v>28.401191658391259</v>
       </c>
     </row>
-    <row r="429" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>27</v>
       </c>
@@ -10917,7 +10917,7 @@
         <v>26.812313803376366</v>
       </c>
     </row>
-    <row r="430" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>27</v>
       </c>
@@ -10941,7 +10941,7 @@
         <v>27.408142999006952</v>
       </c>
     </row>
-    <row r="431" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>27</v>
       </c>
@@ -10965,7 +10965,7 @@
         <v>28.713474025974026</v>
       </c>
     </row>
-    <row r="432" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>27</v>
       </c>
@@ -10986,7 +10986,7 @@
       </c>
       <c r="H432" s="5"/>
     </row>
-    <row r="433" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>27</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>28.300019790223629</v>
       </c>
     </row>
-    <row r="434" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>27</v>
       </c>
@@ -11034,7 +11034,7 @@
         <v>28.579994004197061</v>
       </c>
     </row>
-    <row r="435" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>27</v>
       </c>
@@ -11058,7 +11058,7 @@
         <v>30.468347915594443</v>
       </c>
     </row>
-    <row r="436" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>27</v>
       </c>
@@ -11082,7 +11082,7 @@
         <v>26.246719160104984</v>
       </c>
     </row>
-    <row r="437" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>27</v>
       </c>
@@ -11106,7 +11106,7 @@
         <v>26.061057334326136</v>
       </c>
     </row>
-    <row r="438" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
         <v>27</v>
       </c>
@@ -11130,7 +11130,7 @@
         <v>25.220550077841203</v>
       </c>
     </row>
-    <row r="439" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>27</v>
       </c>
@@ -11154,7 +11154,7 @@
         <v>25.328137817883508</v>
       </c>
     </row>
-    <row r="440" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>27</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>25.509154494959887</v>
       </c>
     </row>
-    <row r="441" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>27</v>
       </c>
@@ -11202,7 +11202,7 @@
         <v>26.30497328401151</v>
       </c>
     </row>
-    <row r="442" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>27</v>
       </c>
@@ -11226,7 +11226,7 @@
         <v>26.034163408108665</v>
       </c>
     </row>
-    <row r="443" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>27</v>
       </c>
@@ -11250,7 +11250,7 @@
         <v>25.194592380172061</v>
       </c>
     </row>
-    <row r="444" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
         <v>27</v>
       </c>
@@ -11274,7 +11274,7 @@
         <v>25.42709574890743</v>
       </c>
     </row>
-    <row r="445" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
         <v>27</v>
       </c>
@@ -11298,7 +11298,7 @@
         <v>27.239908106334099</v>
       </c>
     </row>
-    <row r="446" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>27</v>
       </c>
@@ -11322,7 +11322,7 @@
         <v>25.779376498800961</v>
       </c>
     </row>
-    <row r="447" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>27</v>
       </c>
@@ -11346,7 +11346,7 @@
         <v>25.17412935323383</v>
       </c>
     </row>
-    <row r="448" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
         <v>27</v>
       </c>
@@ -11370,7 +11370,7 @@
         <v>25.17412935323383</v>
       </c>
     </row>
-    <row r="449" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
         <v>27</v>
       </c>
@@ -11394,7 +11394,7 @@
         <v>24.088879659433079</v>
       </c>
     </row>
-    <row r="450" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
         <v>27</v>
       </c>
@@ -11418,7 +11418,7 @@
         <v>24.151696606786427</v>
       </c>
     </row>
-    <row r="451" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
         <v>27</v>
       </c>
@@ -11442,7 +11442,7 @@
         <v>25.166543301258326</v>
       </c>
     </row>
-    <row r="452" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
         <v>27</v>
       </c>
@@ -11466,7 +11466,7 @@
         <v>24.881760230310505</v>
       </c>
     </row>
-    <row r="453" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
         <v>27</v>
       </c>
@@ -11490,7 +11490,7 @@
         <v>25.119617224880383</v>
       </c>
     </row>
-    <row r="454" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
         <v>27</v>
       </c>
@@ -11514,7 +11514,7 @@
         <v>24.820574162679424</v>
       </c>
     </row>
-    <row r="455" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
         <v>27</v>
       </c>
@@ -11538,7 +11538,7 @@
         <v>24.12280701754386</v>
       </c>
     </row>
-    <row r="456" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
         <v>27</v>
       </c>
@@ -11559,7 +11559,7 @@
       </c>
       <c r="H456" s="5"/>
     </row>
-    <row r="457" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
         <v>27</v>
       </c>
@@ -11583,7 +11583,7 @@
         <v>25.715204114432659</v>
       </c>
     </row>
-    <row r="458" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
         <v>27</v>
       </c>
@@ -11607,7 +11607,7 @@
         <v>26.258705331658863</v>
       </c>
     </row>
-    <row r="459" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
         <v>27</v>
       </c>
@@ -11631,7 +11631,7 @@
         <v>25.543992431409649</v>
       </c>
     </row>
-    <row r="460" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
         <v>27</v>
       </c>
@@ -11655,7 +11655,7 @@
         <v>25.826446280991735</v>
       </c>
     </row>
-    <row r="461" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>27</v>
       </c>
@@ -11679,7 +11679,7 @@
         <v>28.479638794825043</v>
       </c>
     </row>
-    <row r="462" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
         <v>27</v>
       </c>
@@ -11703,7 +11703,7 @@
         <v>26.637931034482758</v>
       </c>
     </row>
-    <row r="463" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>27</v>
       </c>
@@ -11727,7 +11727,7 @@
         <v>27.738442315701789</v>
       </c>
     </row>
-    <row r="464" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>27</v>
       </c>
@@ -11751,7 +11751,7 @@
         <v>28.154935443565179</v>
       </c>
     </row>
-    <row r="465" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>27</v>
       </c>
@@ -11775,7 +11775,7 @@
         <v>28.014513543160913</v>
       </c>
     </row>
-    <row r="466" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>27</v>
       </c>
@@ -11799,7 +11799,7 @@
         <v>27.405247813411076</v>
       </c>
     </row>
-    <row r="467" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>27</v>
       </c>
@@ -11823,7 +11823,7 @@
         <v>28.809325562031642</v>
       </c>
     </row>
-    <row r="468" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
         <v>27</v>
       </c>
@@ -11847,7 +11847,7 @@
         <v>26.954177897574127</v>
       </c>
     </row>
-    <row r="469" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>27</v>
       </c>
@@ -11871,7 +11871,7 @@
         <v>26.587132509586709</v>
       </c>
     </row>
-    <row r="470" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
         <v>27</v>
       </c>
@@ -11895,7 +11895,7 @@
         <v>26.405664306538942</v>
       </c>
     </row>
-    <row r="471" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
         <v>27</v>
       </c>
@@ -11919,7 +11919,7 @@
         <v>27.238000332170735</v>
       </c>
     </row>
-    <row r="472" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
         <v>27</v>
       </c>
@@ -11943,7 +11943,7 @@
         <v>27.486256871564219</v>
       </c>
     </row>
-    <row r="473" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
         <v>27</v>
       </c>
@@ -11967,7 +11967,7 @@
         <v>27.477102414654453</v>
       </c>
     </row>
-    <row r="474" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
         <v>27</v>
       </c>
@@ -11991,7 +11991,7 @@
         <v>26.542800265428003</v>
       </c>
     </row>
-    <row r="475" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
         <v>27</v>
       </c>
@@ -12015,7 +12015,7 @@
         <v>28.607172643869891</v>
       </c>
     </row>
-    <row r="476" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>27</v>
       </c>
@@ -12039,7 +12039,7 @@
         <v>27.905039566847144</v>
       </c>
     </row>
-    <row r="477" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>27</v>
       </c>
@@ -12063,7 +12063,7 @@
         <v>28.895856283365816</v>
       </c>
     </row>
-    <row r="478" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
         <v>27</v>
       </c>
@@ -12087,7 +12087,7 @@
         <v>26.836158192090398</v>
       </c>
     </row>
-    <row r="479" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>27</v>
       </c>
@@ -12111,7 +12111,7 @@
         <v>26.586905948820206</v>
       </c>
     </row>
-    <row r="480" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>27</v>
       </c>
@@ -12135,7 +12135,7 @@
         <v>25.756065137919574</v>
       </c>
     </row>
-    <row r="481" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>27</v>
       </c>
@@ -12159,7 +12159,7 @@
         <v>28.079242032730406</v>
       </c>
     </row>
-    <row r="482" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>27</v>
       </c>
@@ -12180,7 +12180,7 @@
       </c>
       <c r="H482" s="5"/>
     </row>
-    <row r="483" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>27</v>
       </c>
@@ -12204,7 +12204,7 @@
         <v>26.168224299065422</v>
       </c>
     </row>
-    <row r="484" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>27</v>
       </c>
@@ -12228,7 +12228,7 @@
         <v>26.7455424095984</v>
       </c>
     </row>
-    <row r="485" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>27</v>
       </c>
@@ -12252,7 +12252,7 @@
         <v>27.072053311120364</v>
       </c>
     </row>
-    <row r="486" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
         <v>27</v>
       </c>
@@ -12276,7 +12276,7 @@
         <v>3.5788597586350392</v>
       </c>
     </row>
-    <row r="487" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>27</v>
       </c>
@@ -12300,7 +12300,7 @@
         <v>25.908030656447853</v>
       </c>
     </row>
-    <row r="488" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
         <v>27</v>
       </c>
@@ -12324,7 +12324,7 @@
         <v>25.86923972716686</v>
       </c>
     </row>
-    <row r="489" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
         <v>27</v>
       </c>
@@ -12348,7 +12348,7 @@
         <v>27.388922702373709</v>
       </c>
     </row>
-    <row r="490" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
         <v>27</v>
       </c>
@@ -12372,7 +12372,7 @@
         <v>25.939026444332153</v>
       </c>
     </row>
-    <row r="491" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
         <v>27</v>
       </c>
@@ -12396,7 +12396,7 @@
         <v>26.285143902844784</v>
       </c>
     </row>
-    <row r="492" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>27</v>
       </c>
@@ -12420,7 +12420,7 @@
         <v>27.132750728256344</v>
       </c>
     </row>
-    <row r="493" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>27</v>
       </c>
@@ -12444,7 +12444,7 @@
         <v>25.07288629737609</v>
       </c>
     </row>
-    <row r="494" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>27</v>
       </c>
@@ -12468,7 +12468,7 @@
         <v>26.611820013431831</v>
       </c>
     </row>
-    <row r="495" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>27</v>
       </c>
@@ -12492,7 +12492,7 @@
         <v>26.975272666722173</v>
       </c>
     </row>
-    <row r="496" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>27</v>
       </c>
@@ -12516,7 +12516,7 @@
         <v>26.953060208989882</v>
       </c>
     </row>
-    <row r="497" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>27</v>
       </c>
@@ -12540,7 +12540,7 @@
         <v>27.159876697492294</v>
       </c>
     </row>
-    <row r="498" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>27</v>
       </c>
@@ -12564,7 +12564,7 @@
         <v>27.159876697492294</v>
       </c>
     </row>
-    <row r="499" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>27</v>
       </c>
@@ -12588,7 +12588,7 @@
         <v>28.198653198653197</v>
       </c>
     </row>
-    <row r="500" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>27</v>
       </c>
@@ -12612,7 +12612,7 @@
         <v>28.476269775187344</v>
       </c>
     </row>
-    <row r="501" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>27</v>
       </c>
@@ -12636,7 +12636,7 @@
         <v>28.813705979060309</v>
       </c>
     </row>
-    <row r="502" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>27</v>
       </c>
@@ -12660,7 +12660,7 @@
         <v>28.02130274477673</v>
       </c>
     </row>
-    <row r="503" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>27</v>
       </c>
@@ -12684,7 +12684,7 @@
         <v>28.132780082987551</v>
       </c>
     </row>
-    <row r="504" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>27</v>
       </c>
@@ -12708,7 +12708,7 @@
         <v>27.883817427385889</v>
       </c>
     </row>
-    <row r="505" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>27</v>
       </c>
@@ -12732,7 +12732,7 @@
         <v>27.385892116182571</v>
       </c>
     </row>
-    <row r="506" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>27</v>
       </c>
@@ -12756,7 +12756,7 @@
         <v>27.905039566847144</v>
       </c>
     </row>
-    <row r="507" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>27</v>
       </c>
@@ -12777,7 +12777,7 @@
       </c>
       <c r="H507" s="5"/>
     </row>
-    <row r="508" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>27</v>
       </c>
@@ -12801,7 +12801,7 @@
         <v>28.141199703776845</v>
       </c>
     </row>
-    <row r="509" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>27</v>
       </c>
@@ -12825,7 +12825,7 @@
         <v>27.35112936344969</v>
       </c>
     </row>
-    <row r="510" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>27</v>
       </c>
@@ -12849,7 +12849,7 @@
         <v>28.269419862340214</v>
       </c>
     </row>
-    <row r="511" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>27</v>
       </c>
@@ -12873,7 +12873,7 @@
         <v>27.695837430350704</v>
       </c>
     </row>
-    <row r="512" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
         <v>27</v>
       </c>
@@ -12897,7 +12897,7 @@
         <v>26.33436498886898</v>
       </c>
     </row>
-    <row r="513" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>27</v>
       </c>
@@ -12921,7 +12921,7 @@
         <v>25.334654124990138</v>
       </c>
     </row>
-    <row r="514" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>27</v>
       </c>
@@ -12945,7 +12945,7 @@
         <v>25.522648083623693</v>
       </c>
     </row>
-    <row r="515" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>27</v>
       </c>
@@ -12969,7 +12969,7 @@
         <v>25.195482189400522</v>
       </c>
     </row>
-    <row r="516" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>27</v>
       </c>
@@ -12993,7 +12993,7 @@
         <v>25.530110262934691</v>
       </c>
     </row>
-    <row r="517" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
         <v>27</v>
       </c>
@@ -13017,7 +13017,7 @@
         <v>24.979184013322232</v>
       </c>
     </row>
-    <row r="518" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
         <v>27</v>
       </c>
@@ -13041,7 +13041,7 @@
         <v>25.62320854686007</v>
       </c>
     </row>
-    <row r="519" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
         <v>27</v>
       </c>
@@ -13065,7 +13065,7 @@
         <v>25.297748413457359</v>
       </c>
     </row>
-    <row r="520" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
         <v>27</v>
       </c>
@@ -13089,7 +13089,7 @@
         <v>25.169409486931269</v>
       </c>
     </row>
-    <row r="521" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
         <v>27</v>
       </c>
@@ -13113,7 +13113,7 @@
         <v>24.900066622251835</v>
       </c>
     </row>
-    <row r="522" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
         <v>27</v>
       </c>
@@ -13137,7 +13137,7 @@
         <v>25.062447960033307</v>
       </c>
     </row>
-    <row r="523" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A523" t="s">
         <v>27</v>
       </c>
@@ -13161,7 +13161,7 @@
         <v>25.081243229730855</v>
       </c>
     </row>
-    <row r="524" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A524" t="s">
         <v>27</v>
       </c>
@@ -13185,7 +13185,7 @@
         <v>23.664694608782604</v>
       </c>
     </row>
-    <row r="525" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A525" t="s">
         <v>27</v>
       </c>
@@ -13209,7 +13209,7 @@
         <v>22.674611055941742</v>
       </c>
     </row>
-    <row r="526" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A526" t="s">
         <v>27</v>
       </c>
@@ -13233,7 +13233,7 @@
         <v>23.636363636363637</v>
       </c>
     </row>
-    <row r="527" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
         <v>27</v>
       </c>
@@ -13257,7 +13257,7 @@
         <v>25.2423938482113</v>
       </c>
     </row>
-    <row r="528" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A528" t="s">
         <v>27</v>
       </c>
@@ -13281,7 +13281,7 @@
         <v>24.995834027662056</v>
       </c>
     </row>
-    <row r="529" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
         <v>27</v>
       </c>
@@ -13305,7 +13305,7 @@
         <v>24.20965058236273</v>
       </c>
     </row>
-    <row r="530" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
         <v>27</v>
       </c>
@@ -13329,7 +13329,7 @@
         <v>22.795341098169718</v>
       </c>
     </row>
-    <row r="531" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
         <v>27</v>
       </c>
@@ -13353,7 +13353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="532" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
         <v>27</v>
       </c>
@@ -13377,7 +13377,7 @@
         <v>24.511082138200781</v>
       </c>
     </row>
-    <row r="533" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>27</v>
       </c>
@@ -13401,7 +13401,7 @@
         <v>23.632271468144044</v>
       </c>
     </row>
-    <row r="534" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
         <v>27</v>
       </c>
@@ -13425,7 +13425,7 @@
         <v>23.950103950103948</v>
       </c>
     </row>
-    <row r="535" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>27</v>
       </c>
@@ -18418,13 +18418,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H742" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="JJMLN"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H742" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E537:E1048576 E1:E535 M160:M166" xr:uid="{C0D40973-6001-441E-B08C-5897C12BA20E}">

</xml_diff>